<commit_message>
docs: add sone test file
</commit_message>
<xml_diff>
--- a/python/mutual_mold/files/04.PT. FUJI SEAT.xlsx
+++ b/python/mutual_mold/files/04.PT. FUJI SEAT.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\go\src\practice\python\mutual_mold\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F303F64-BC98-4CB5-9CA7-BC1A2E22B175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LIST MOLD 1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,20 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'LIST MOLD 1'!$A$1:$R$17</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'LIST MOLD 2'!$A$1:$Q$18</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -26,7 +45,7 @@
         <b/>
         <sz val="18"/>
         <rFont val="Trebuchet MS"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">LIST PART/MOLD                                                                   </t>
     </r>
@@ -36,7 +55,7 @@
         <sz val="18"/>
         <color indexed="12"/>
         <rFont val="Trebuchet MS"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>CUSTOMOR PT.FUJI SEAT MODEL D74A</t>
     </r>
@@ -189,15 +208,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-&quot;NT$&quot;* #,##0.00_-;\-&quot;NT$&quot;* #,##0.00_-;_-&quot;NT$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;NT$&quot;* #,##0_-;\-&quot;NT$&quot;* #,##0_-;_-&quot;NT$&quot;* &quot;-&quot;_-;_-@_-"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
     <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
@@ -206,190 +221,45 @@
     <font>
       <sz val="12"/>
       <name val="Trebuchet MS"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Trebuchet MS"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Trebuchet MS"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <name val="Trebuchet MS"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial Cyr"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color indexed="12"/>
       <name val="Trebuchet MS"/>
-      <charset val="134"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -402,194 +272,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="35">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -907,263 +591,21 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1172,29 +614,251 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1202,319 +866,95 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="49" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="50">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
-    <cellStyle name="Style 1" xfId="49"/>
+  <cellStyles count="2">
+    <cellStyle name="Style 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -1530,20 +970,32 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="Group 1134"/>
+        <xdr:cNvPr id="2" name="Group 1134">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="200025" y="361950"/>
-          <a:ext cx="2066925" cy="704850"/>
+          <a:off x="202266" y="358588"/>
+          <a:ext cx="2063003" cy="697006"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="2162825" cy="773091"/>
         </a:xfrm>
       </xdr:grpSpPr>
-      <xdr:sp>
+      <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="WordArt 69"/>
+          <xdr:cNvPr id="3" name="WordArt 69">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1" noChangeShapeType="1" noTextEdit="1"/>
           </xdr:cNvSpPr>
@@ -1592,27 +1044,24 @@
               </a:rPr>
               <a:t>PT. YUJU INDONESIA</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="3600" kern="10" spc="0">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:srgbClr val="333399"/>
-              </a:solidFill>
-              <a:latin typeface="Arial Black" panose="020B0A04020102020204"/>
-            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="4" name="Picture 360"/>
+          <xdr:cNvPr id="4" name="Picture 360">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip r:embed="rId1" cstate="print">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
             <a:extLst>
               <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
                 <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1664,7 +1113,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1680,20 +1129,32 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="Group 1134"/>
+        <xdr:cNvPr id="2" name="Group 1134">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="267970" y="103505"/>
-          <a:ext cx="3324860" cy="822325"/>
+          <a:off x="268320" y="103470"/>
+          <a:ext cx="3325091" cy="828079"/>
           <a:chOff x="90518" y="68185"/>
           <a:chExt cx="2072307" cy="676962"/>
         </a:xfrm>
       </xdr:grpSpPr>
-      <xdr:sp>
+      <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="WordArt 69"/>
+          <xdr:cNvPr id="3" name="WordArt 69">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeArrowheads="1" noChangeShapeType="1" noTextEdit="1"/>
           </xdr:cNvSpPr>
@@ -1742,27 +1203,24 @@
               </a:rPr>
               <a:t>PT. YUJU INDONESIA</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="3600" kern="10" spc="0">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:srgbClr val="333399"/>
-              </a:solidFill>
-              <a:latin typeface="Arial Black" panose="020B0A04020102020204"/>
-            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="4" name="Picture 360"/>
+          <xdr:cNvPr id="4" name="Picture 360">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip r:embed="rId1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
             <a:extLst>
               <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
                 <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2065,16 +1523,16 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R17"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A1" sqref="A$1:A$1048576"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
@@ -3166,549 +2624,518 @@
     <col min="16139" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="5.25" customHeight="1"/>
-    <row r="2" ht="23.25" customHeight="1" spans="2:18">
+    <row r="1" spans="2:18" ht="5.25" customHeight="1"/>
+    <row r="2" spans="2:18" ht="23.25" customHeight="1">
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="84"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="53" t="s">
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="54"/>
-      <c r="O2" s="53" t="s">
+      <c r="N2" s="35"/>
+      <c r="O2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="38"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="25"/>
     </row>
-    <row r="3" ht="23.25" customHeight="1" spans="2:18">
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="53" t="s">
+    <row r="3" spans="2:18" ht="23.25" customHeight="1">
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="54"/>
-      <c r="O3" s="53" t="s">
+      <c r="N3" s="35"/>
+      <c r="O3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="38"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="25"/>
     </row>
-    <row r="4" ht="23.25" customHeight="1" spans="2:18">
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="53" t="s">
+    <row r="4" spans="2:18" ht="23.25" customHeight="1">
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="54"/>
-      <c r="O4" s="53" t="s">
+      <c r="N4" s="35"/>
+      <c r="O4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="55"/>
-      <c r="Q4" s="55"/>
-      <c r="R4" s="38"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="25"/>
     </row>
-    <row r="5" ht="23.25" customHeight="1" spans="2:18">
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="57"/>
-      <c r="M5" s="53" t="s">
+    <row r="5" spans="2:18" ht="23.25" customHeight="1">
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="91"/>
+      <c r="L5" s="92"/>
+      <c r="M5" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="54"/>
-      <c r="O5" s="53" t="s">
+      <c r="N5" s="35"/>
+      <c r="O5" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="55"/>
-      <c r="Q5" s="55"/>
-      <c r="R5" s="38"/>
+      <c r="P5" s="36"/>
+      <c r="Q5" s="36"/>
+      <c r="R5" s="25"/>
     </row>
-    <row r="6" ht="18.75" customHeight="1" spans="2:18">
-      <c r="B6" s="21" t="s">
+    <row r="6" spans="2:18" ht="18.75" customHeight="1">
+      <c r="B6" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="94"/>
+      <c r="E6" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="22" t="s">
+      <c r="F6" s="94"/>
+      <c r="G6" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="58" t="s">
+      <c r="K6" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="59"/>
-      <c r="M6" s="21" t="s">
+      <c r="L6" s="55"/>
+      <c r="M6" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="60" t="s">
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" s="58" t="s">
+      <c r="Q6" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="R6" s="59"/>
+      <c r="R6" s="55"/>
     </row>
-    <row r="7" ht="18.75" customHeight="1" spans="2:18">
-      <c r="B7" s="25"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="63"/>
-      <c r="M7" s="25" t="s">
+    <row r="7" spans="2:18" ht="18.75" customHeight="1">
+      <c r="B7" s="77"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="97"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="N7" s="25" t="s">
+      <c r="N7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="O7" s="25" t="s">
+      <c r="O7" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="P7" s="64"/>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="63"/>
+      <c r="P7" s="83"/>
+      <c r="Q7" s="97"/>
+      <c r="R7" s="98"/>
     </row>
-    <row r="8" ht="98.1" customHeight="1" spans="2:18">
-      <c r="B8" s="30">
+    <row r="8" spans="2:18" ht="98.1" customHeight="1">
+      <c r="B8" s="19">
         <v>1</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="36" t="s">
+      <c r="D8" s="48"/>
+      <c r="E8" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="55"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="35" t="s">
+      <c r="F8" s="50"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="69">
+      <c r="J8" s="38">
         <v>1</v>
       </c>
-      <c r="K8" s="70" t="s">
+      <c r="K8" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="71"/>
-      <c r="M8" s="21">
+      <c r="L8" s="52"/>
+      <c r="M8" s="15">
         <v>600</v>
       </c>
-      <c r="N8" s="21">
+      <c r="N8" s="15">
         <v>490</v>
       </c>
-      <c r="O8" s="21">
+      <c r="O8" s="15">
         <v>390</v>
       </c>
-      <c r="P8" s="21">
+      <c r="P8" s="15">
         <v>670</v>
       </c>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="38"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="53"/>
     </row>
-    <row r="9" ht="98.1" customHeight="1" spans="2:18">
-      <c r="B9" s="21">
+    <row r="9" spans="2:18" ht="98.1" customHeight="1">
+      <c r="B9" s="15">
         <f>+B8+1</f>
         <v>2</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="59"/>
-      <c r="E9" s="36" t="s">
+      <c r="D9" s="55"/>
+      <c r="E9" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="38"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="69">
+      <c r="F9" s="53"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="38">
         <v>1</v>
       </c>
-      <c r="K9" s="70" t="s">
+      <c r="K9" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="71"/>
-      <c r="M9" s="21">
+      <c r="L9" s="52"/>
+      <c r="M9" s="15">
         <v>600</v>
       </c>
-      <c r="N9" s="21">
+      <c r="N9" s="15">
         <v>490</v>
       </c>
-      <c r="O9" s="21">
+      <c r="O9" s="15">
         <v>390</v>
       </c>
-      <c r="P9" s="21">
+      <c r="P9" s="15">
         <v>670</v>
       </c>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="38"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="53"/>
     </row>
-    <row r="10" ht="85.5" customHeight="1" spans="2:18">
-      <c r="B10" s="21">
+    <row r="10" spans="2:18" ht="85.5" customHeight="1">
+      <c r="B10" s="15">
         <f>+B9+1</f>
         <v>3</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="93"/>
-      <c r="J10" s="94"/>
-      <c r="K10" s="70"/>
-      <c r="L10" s="71"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="38"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="53"/>
     </row>
-    <row r="11" ht="85.5" customHeight="1" spans="2:18">
-      <c r="B11" s="21">
+    <row r="11" spans="2:18" ht="85.5" customHeight="1">
+      <c r="B11" s="15">
         <f>+B10+1</f>
         <v>4</v>
       </c>
-      <c r="C11" s="86"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="89"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="93"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="95"/>
-      <c r="L11" s="96"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="86"/>
-      <c r="R11" s="87"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="61"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="56"/>
+      <c r="R11" s="57"/>
     </row>
-    <row r="12" s="1" customFormat="1" ht="98.1" customHeight="1" spans="2:18">
-      <c r="B12" s="30">
+    <row r="12" spans="2:18" ht="98.1" customHeight="1">
+      <c r="B12" s="19">
         <v>1</v>
       </c>
-      <c r="C12" s="90" t="s">
+      <c r="C12" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="91"/>
-      <c r="E12" s="31" t="s">
+      <c r="D12" s="63"/>
+      <c r="E12" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="92"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="35" t="s">
+      <c r="F12" s="65"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="72">
+      <c r="J12" s="39">
         <v>2</v>
       </c>
       <c r="K12" s="66" t="s">
         <v>32</v>
       </c>
       <c r="L12" s="67"/>
-      <c r="M12" s="34">
+      <c r="M12" s="22">
         <v>550</v>
       </c>
-      <c r="N12" s="34">
+      <c r="N12" s="22">
         <v>550</v>
       </c>
-      <c r="O12" s="34">
+      <c r="O12" s="22">
         <v>480</v>
       </c>
-      <c r="P12" s="34">
+      <c r="P12" s="22">
         <v>920</v>
       </c>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="92"/>
+      <c r="Q12" s="64"/>
+      <c r="R12" s="65"/>
     </row>
-    <row r="13" s="1" customFormat="1" ht="98.1" customHeight="1" spans="2:18">
-      <c r="B13" s="21">
+    <row r="13" spans="2:18" ht="98.1" customHeight="1">
+      <c r="B13" s="15">
         <f>+B12+1</f>
         <v>2</v>
       </c>
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="59"/>
-      <c r="E13" s="43" t="s">
+      <c r="D13" s="55"/>
+      <c r="E13" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="44"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="69">
+      <c r="F13" s="48"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="38">
         <v>2</v>
       </c>
-      <c r="K13" s="70" t="s">
+      <c r="K13" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="L13" s="71"/>
-      <c r="M13" s="21">
+      <c r="L13" s="52"/>
+      <c r="M13" s="15">
         <v>550</v>
       </c>
-      <c r="N13" s="21">
+      <c r="N13" s="15">
         <v>550</v>
       </c>
-      <c r="O13" s="21">
+      <c r="O13" s="15">
         <v>480</v>
       </c>
-      <c r="P13" s="21">
+      <c r="P13" s="15">
         <v>920</v>
       </c>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="38"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="53"/>
     </row>
-    <row r="14" s="1" customFormat="1" ht="98.1" customHeight="1" spans="2:18">
-      <c r="B14" s="21">
+    <row r="14" spans="2:18" ht="98.1" customHeight="1">
+      <c r="B14" s="15">
         <f>+B13+1</f>
         <v>3</v>
       </c>
-      <c r="C14" s="58" t="s">
+      <c r="C14" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="60"/>
-      <c r="E14" s="43" t="s">
+      <c r="D14" s="68"/>
+      <c r="E14" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="44"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="69">
+      <c r="F14" s="48"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="38">
         <v>4</v>
       </c>
-      <c r="K14" s="70" t="s">
+      <c r="K14" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="71"/>
-      <c r="M14" s="21">
+      <c r="L14" s="52"/>
+      <c r="M14" s="15">
         <v>500</v>
       </c>
-      <c r="N14" s="21">
+      <c r="N14" s="15">
         <v>430</v>
       </c>
-      <c r="O14" s="21">
+      <c r="O14" s="15">
         <v>410</v>
       </c>
-      <c r="P14" s="21">
+      <c r="P14" s="15">
         <v>590</v>
       </c>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="38"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="53"/>
     </row>
-    <row r="15" s="1" customFormat="1" ht="98.1" customHeight="1" spans="2:18">
-      <c r="B15" s="21">
+    <row r="15" spans="2:18" ht="98.1" customHeight="1">
+      <c r="B15" s="15">
         <f>+B14+1</f>
         <v>4</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="43" t="s">
+      <c r="D15" s="48"/>
+      <c r="E15" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="44"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="69">
+      <c r="F15" s="48"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="38">
         <v>2</v>
       </c>
-      <c r="K15" s="70" t="s">
+      <c r="K15" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="L15" s="71"/>
-      <c r="M15" s="21">
+      <c r="L15" s="52"/>
+      <c r="M15" s="15">
         <v>560</v>
       </c>
-      <c r="N15" s="21">
+      <c r="N15" s="15">
         <v>590</v>
       </c>
-      <c r="O15" s="21">
+      <c r="O15" s="15">
         <v>540</v>
       </c>
-      <c r="P15" s="21">
+      <c r="P15" s="15">
         <v>1456</v>
       </c>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="38"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="53"/>
     </row>
-    <row r="16" s="1" customFormat="1" ht="76.5" customHeight="1" spans="2:18">
-      <c r="B16" s="21">
+    <row r="16" spans="2:18" ht="76.5" customHeight="1">
+      <c r="B16" s="15">
         <v>5</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="44"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="45"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="29"/>
       <c r="J16" s="1">
         <v>8</v>
       </c>
-      <c r="K16" s="76" t="s">
+      <c r="K16" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="L16" s="77"/>
-      <c r="M16" s="21">
+      <c r="L16" s="70"/>
+      <c r="M16" s="15">
         <v>900</v>
       </c>
-      <c r="N16" s="21">
+      <c r="N16" s="15">
         <v>850</v>
       </c>
-      <c r="O16" s="21">
+      <c r="O16" s="15">
         <v>500</v>
       </c>
-      <c r="P16" s="21">
+      <c r="P16" s="15">
         <v>2237</v>
       </c>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="38"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="25"/>
     </row>
-    <row r="17" s="1" customFormat="1" ht="81.75" customHeight="1" spans="2:18">
-      <c r="B17" s="46">
+    <row r="17" spans="2:18" ht="81.75" customHeight="1">
+      <c r="B17" s="30">
         <v>6</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="50"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="78">
+      <c r="D17" s="72"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="41">
         <v>2</v>
       </c>
-      <c r="K17" s="79" t="s">
+      <c r="K17" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="L17" s="80"/>
-      <c r="M17" s="46">
+      <c r="L17" s="74"/>
+      <c r="M17" s="30">
         <v>600</v>
       </c>
-      <c r="N17" s="46">
+      <c r="N17" s="30">
         <v>330</v>
       </c>
-      <c r="O17" s="46">
+      <c r="O17" s="30">
         <v>400</v>
       </c>
-      <c r="P17" s="46">
+      <c r="P17" s="30">
         <v>494</v>
       </c>
-      <c r="Q17" s="47"/>
-      <c r="R17" s="97"/>
+      <c r="Q17" s="75"/>
+      <c r="R17" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="F2:L5"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="E6:F7"/>
+    <mergeCell ref="K6:L7"/>
+    <mergeCell ref="Q6:R7"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="K17:L17"/>
@@ -3721,35 +3148,69 @@
     <mergeCell ref="I12:I15"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="P6:P7"/>
-    <mergeCell ref="F2:L5"/>
-    <mergeCell ref="C6:D7"/>
-    <mergeCell ref="E6:F7"/>
-    <mergeCell ref="K6:L7"/>
-    <mergeCell ref="Q6:R7"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="Q8:R8"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.156944444444444" top="0.275" bottom="0.393055555555556" header="0" footer="0"/>
-  <pageSetup paperSize="5" scale="80" fitToHeight="8" orientation="landscape"/>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.25" right="0.156944444444444" top="0.27500000000000002" bottom="0.39305555555555599" header="0" footer="0"/>
+  <pageSetup paperSize="5" scale="80" fitToHeight="8" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:Q18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="7" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="4.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.15" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.125" style="2" customWidth="1"/>
     <col min="4" max="4" width="8.25" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.375" style="1" customWidth="1"/>
     <col min="6" max="6" width="23.375" style="1" customWidth="1"/>
@@ -4833,614 +4294,618 @@
     <col min="16138" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="5.25" customHeight="1"/>
-    <row r="2" ht="23.25" customHeight="1" spans="1:17">
+    <row r="1" spans="1:17" ht="5.25" customHeight="1">
+      <c r="P1" s="99"/>
+      <c r="Q1" s="99"/>
+    </row>
+    <row r="2" spans="1:17" ht="23.25" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="53" t="s">
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="54"/>
-      <c r="N2" s="53" t="s">
+      <c r="M2" s="35"/>
+      <c r="N2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="55"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="100"/>
+      <c r="Q2" s="100"/>
     </row>
-    <row r="3" ht="23.25" customHeight="1" spans="1:17">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="53" t="s">
+    <row r="3" spans="1:17" ht="23.25" customHeight="1">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="54"/>
-      <c r="N3" s="53" t="s">
+      <c r="M3" s="35"/>
+      <c r="N3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="55"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="100"/>
     </row>
-    <row r="4" ht="23.25" customHeight="1" spans="1:17">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="53" t="s">
+    <row r="4" spans="1:17" ht="23.25" customHeight="1">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="54"/>
-      <c r="N4" s="53" t="s">
+      <c r="M4" s="35"/>
+      <c r="N4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="55"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="100"/>
+      <c r="Q4" s="100"/>
     </row>
-    <row r="5" ht="23.25" customHeight="1" spans="1:17">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="57"/>
-      <c r="L5" s="53" t="s">
+    <row r="5" spans="1:17" ht="23.25" customHeight="1">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="54"/>
-      <c r="N5" s="53" t="s">
+      <c r="M5" s="35"/>
+      <c r="N5" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="O5" s="55"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="100"/>
+      <c r="Q5" s="100"/>
     </row>
-    <row r="6" ht="18.75" customHeight="1" spans="1:17">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:17" ht="18.75" customHeight="1">
+      <c r="A6" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="22" t="s">
+      <c r="E6" s="94"/>
+      <c r="F6" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="58" t="s">
+      <c r="J6" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="59"/>
-      <c r="L6" s="21" t="s">
+      <c r="K6" s="55"/>
+      <c r="L6" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="60" t="s">
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="61" t="s">
+      <c r="P6" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="82"/>
+      <c r="Q6" s="102"/>
     </row>
-    <row r="7" ht="18.75" customHeight="1" spans="1:17">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="63"/>
-      <c r="L7" s="25" t="s">
+    <row r="7" spans="1:17" ht="18.75" customHeight="1">
+      <c r="A7" s="77"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="97"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="25" t="s">
+      <c r="M7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="N7" s="25" t="s">
+      <c r="N7" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="O7" s="64"/>
-      <c r="P7" s="61"/>
-      <c r="Q7" s="82"/>
+      <c r="O7" s="83"/>
+      <c r="P7" s="101"/>
+      <c r="Q7" s="102"/>
     </row>
-    <row r="8" ht="98.1" customHeight="1" spans="1:17">
-      <c r="A8" s="30">
+    <row r="8" spans="1:17" ht="98.1" customHeight="1">
+      <c r="A8" s="19">
         <v>1</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="33"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35" t="s">
+      <c r="E8" s="103"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="65">
+      <c r="I8" s="37">
         <v>1</v>
       </c>
       <c r="J8" s="66" t="s">
         <v>26</v>
       </c>
       <c r="K8" s="67"/>
-      <c r="L8" s="34">
+      <c r="L8" s="22">
         <v>600</v>
       </c>
-      <c r="M8" s="34">
+      <c r="M8" s="22">
         <v>490</v>
       </c>
-      <c r="N8" s="34">
+      <c r="N8" s="22">
         <v>390</v>
       </c>
-      <c r="O8" s="34">
+      <c r="O8" s="22">
         <v>670</v>
       </c>
-      <c r="P8" s="68"/>
-      <c r="Q8" s="11"/>
+      <c r="P8" s="104"/>
+      <c r="Q8" s="100"/>
     </row>
-    <row r="9" ht="98.1" customHeight="1" spans="1:17">
-      <c r="A9" s="21">
+    <row r="9" spans="1:17" ht="98.1" customHeight="1">
+      <c r="A9" s="15">
         <f>+A8+1</f>
         <v>2</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="38"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="69">
+      <c r="E9" s="53"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="38">
         <v>1</v>
       </c>
-      <c r="J9" s="70" t="s">
+      <c r="J9" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="71"/>
-      <c r="L9" s="21">
+      <c r="K9" s="52"/>
+      <c r="L9" s="15">
         <v>600</v>
       </c>
-      <c r="M9" s="21">
+      <c r="M9" s="15">
         <v>490</v>
       </c>
-      <c r="N9" s="21">
+      <c r="N9" s="15">
         <v>390</v>
       </c>
-      <c r="O9" s="21">
+      <c r="O9" s="15">
         <v>670</v>
       </c>
-      <c r="P9" s="68"/>
-      <c r="Q9" s="11"/>
+      <c r="P9" s="104"/>
+      <c r="Q9" s="100"/>
     </row>
-    <row r="10" s="1" customFormat="1" ht="98.1" customHeight="1" spans="1:17">
-      <c r="A10" s="30">
+    <row r="10" spans="1:17" ht="98.1" customHeight="1">
+      <c r="A10" s="19">
         <v>3</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="41" t="s">
+      <c r="E10" s="106"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="72">
+      <c r="I10" s="39">
         <v>2</v>
       </c>
-      <c r="J10" s="73" t="s">
+      <c r="J10" s="107" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="74"/>
-      <c r="L10" s="30">
+      <c r="K10" s="108"/>
+      <c r="L10" s="19">
         <v>550</v>
       </c>
-      <c r="M10" s="30">
+      <c r="M10" s="19">
         <v>550</v>
       </c>
-      <c r="N10" s="30">
+      <c r="N10" s="19">
         <v>480</v>
       </c>
-      <c r="O10" s="30">
+      <c r="O10" s="19">
         <v>920</v>
       </c>
-      <c r="P10" s="68"/>
-      <c r="Q10" s="11"/>
+      <c r="P10" s="104"/>
+      <c r="Q10" s="100"/>
     </row>
-    <row r="11" s="1" customFormat="1" ht="98.1" customHeight="1" spans="1:17">
-      <c r="A11" s="22">
+    <row r="11" spans="1:17" ht="98.1" customHeight="1">
+      <c r="A11" s="78">
         <f>+A10+1</f>
         <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="44"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="69">
+      <c r="E11" s="48"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="38">
         <v>2</v>
       </c>
-      <c r="J11" s="70" t="s">
+      <c r="J11" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="71"/>
-      <c r="L11" s="21">
+      <c r="K11" s="52"/>
+      <c r="L11" s="15">
         <v>550</v>
       </c>
-      <c r="M11" s="21">
+      <c r="M11" s="15">
         <v>550</v>
       </c>
-      <c r="N11" s="21">
+      <c r="N11" s="15">
         <v>480</v>
       </c>
-      <c r="O11" s="21">
+      <c r="O11" s="15">
         <v>920</v>
       </c>
-      <c r="P11" s="68"/>
-      <c r="Q11" s="11"/>
+      <c r="P11" s="104"/>
+      <c r="Q11" s="100"/>
     </row>
-    <row r="12" s="1" customFormat="1" ht="98.1" customHeight="1" spans="1:17">
-      <c r="A12" s="30"/>
+    <row r="12" spans="1:17" ht="98.1" customHeight="1">
+      <c r="A12" s="111"/>
       <c r="B12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="43" t="s">
+      <c r="C12" s="24"/>
+      <c r="D12" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="44"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="68"/>
-      <c r="Q12" s="11"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="104"/>
+      <c r="Q12" s="100"/>
     </row>
-    <row r="13" s="1" customFormat="1" ht="98.1" customHeight="1" spans="1:17">
-      <c r="A13" s="22">
+    <row r="13" spans="1:17" ht="98.1" customHeight="1">
+      <c r="A13" s="78">
         <f>+A11+1</f>
         <v>5</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="44"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="69">
+      <c r="E13" s="48"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="38">
         <v>4</v>
       </c>
-      <c r="J13" s="70" t="s">
+      <c r="J13" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="71"/>
-      <c r="L13" s="21">
+      <c r="K13" s="52"/>
+      <c r="L13" s="15">
         <v>500</v>
       </c>
-      <c r="M13" s="21">
+      <c r="M13" s="15">
         <v>430</v>
       </c>
-      <c r="N13" s="21">
+      <c r="N13" s="15">
         <v>410</v>
       </c>
-      <c r="O13" s="21">
+      <c r="O13" s="15">
         <v>590</v>
       </c>
-      <c r="P13" s="68"/>
-      <c r="Q13" s="11"/>
+      <c r="P13" s="104"/>
+      <c r="Q13" s="100"/>
     </row>
-    <row r="14" s="1" customFormat="1" ht="98.1" customHeight="1" spans="1:17">
-      <c r="A14" s="30"/>
+    <row r="14" spans="1:17" ht="98.1" customHeight="1">
+      <c r="A14" s="111"/>
       <c r="B14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="43" t="s">
+      <c r="C14" s="24"/>
+      <c r="D14" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="44"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="69"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="71"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="68"/>
-      <c r="Q14" s="11"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="104"/>
+      <c r="Q14" s="100"/>
     </row>
-    <row r="15" s="1" customFormat="1" ht="98.1" customHeight="1" spans="1:17">
-      <c r="A15" s="22">
+    <row r="15" spans="1:17" ht="98.1" customHeight="1">
+      <c r="A15" s="78">
         <f>+A13+1</f>
         <v>6</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="44"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="69">
+      <c r="E15" s="48"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="38">
         <v>2</v>
       </c>
-      <c r="J15" s="70" t="s">
+      <c r="J15" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="71"/>
-      <c r="L15" s="21">
+      <c r="K15" s="52"/>
+      <c r="L15" s="15">
         <v>560</v>
       </c>
-      <c r="M15" s="21">
+      <c r="M15" s="15">
         <v>590</v>
       </c>
-      <c r="N15" s="21">
+      <c r="N15" s="15">
         <v>540</v>
       </c>
-      <c r="O15" s="21">
+      <c r="O15" s="15">
         <v>1456</v>
       </c>
-      <c r="P15" s="68"/>
-      <c r="Q15" s="11"/>
+      <c r="P15" s="104"/>
+      <c r="Q15" s="100"/>
     </row>
-    <row r="16" s="1" customFormat="1" ht="98.1" customHeight="1" spans="1:17">
-      <c r="A16" s="30"/>
-      <c r="B16" s="36" t="s">
+    <row r="16" spans="1:17" ht="98.1" customHeight="1">
+      <c r="A16" s="111"/>
+      <c r="B16" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="43" t="s">
+      <c r="C16" s="24"/>
+      <c r="D16" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="44"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="70"/>
-      <c r="K16" s="71"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="68"/>
-      <c r="Q16" s="11"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="104"/>
+      <c r="Q16" s="100"/>
     </row>
-    <row r="17" s="1" customFormat="1" ht="76.5" customHeight="1" spans="1:17">
-      <c r="A17" s="21">
+    <row r="17" spans="1:17" ht="76.5" customHeight="1">
+      <c r="A17" s="15">
         <v>7</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="37" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="43"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="45"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="29"/>
       <c r="I17" s="1">
         <v>8</v>
       </c>
-      <c r="J17" s="76" t="s">
+      <c r="J17" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="77"/>
-      <c r="L17" s="21">
+      <c r="K17" s="70"/>
+      <c r="L17" s="15">
         <v>900</v>
       </c>
-      <c r="M17" s="21">
+      <c r="M17" s="15">
         <v>850</v>
       </c>
-      <c r="N17" s="21">
+      <c r="N17" s="15">
         <v>500</v>
       </c>
-      <c r="O17" s="21">
+      <c r="O17" s="15">
         <v>2237</v>
       </c>
-      <c r="P17" s="68"/>
-      <c r="Q17" s="11"/>
+      <c r="P17" s="104"/>
+      <c r="Q17" s="100"/>
     </row>
-    <row r="18" s="1" customFormat="1" ht="81.75" customHeight="1" spans="1:17">
-      <c r="A18" s="46">
+    <row r="18" spans="1:17" ht="81.75" customHeight="1">
+      <c r="A18" s="30">
         <v>8</v>
       </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="48" t="s">
+      <c r="B18" s="31"/>
+      <c r="C18" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="78">
+      <c r="D18" s="71"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="41">
         <v>2</v>
       </c>
-      <c r="J18" s="79" t="s">
+      <c r="J18" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="K18" s="80"/>
-      <c r="L18" s="46">
+      <c r="K18" s="74"/>
+      <c r="L18" s="30">
         <v>600</v>
       </c>
-      <c r="M18" s="46">
+      <c r="M18" s="30">
         <v>330</v>
       </c>
-      <c r="N18" s="46">
+      <c r="N18" s="30">
         <v>400</v>
       </c>
-      <c r="O18" s="46">
+      <c r="O18" s="30">
         <v>494</v>
       </c>
-      <c r="P18" s="81"/>
-      <c r="Q18" s="83"/>
+      <c r="P18" s="109"/>
+      <c r="Q18" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="E2:K5"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="J6:K7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="H10:H15"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="H8:H9"/>
     <mergeCell ref="L6:N6"/>
     <mergeCell ref="P6:Q6"/>
     <mergeCell ref="P7:Q7"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B6:B7"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H10:H15"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="O6:O7"/>
-    <mergeCell ref="E2:K5"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="J6:K7"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P5:Q5"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.156944444444444" top="0.275" bottom="0.393055555555556" header="0" footer="0"/>
-  <pageSetup paperSize="5" scale="80" fitToHeight="8" orientation="landscape"/>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.25" right="0.156944444444444" top="0.27500000000000002" bottom="0.39305555555555599" header="0" footer="0"/>
+  <pageSetup paperSize="5" scale="80" fitToHeight="8" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>